<commit_message>
rill-analysis: Enhance usability - base on bridge_kpi.xlsx
</commit_message>
<xml_diff>
--- a/rill-analysis/rill-analysis-report-core/src/test/resources/nu/com/rill/analysis/report/excel/bridge_kpi.xlsx
+++ b/rill-analysis/rill-analysis-report-core/src/test/resources/nu/com/rill/analysis/report/excel/bridge_kpi.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="8220"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="8220" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="3" r:id="rId1"/>
@@ -170,7 +170,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1519" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1521" uniqueCount="102">
   <si>
     <t>SELECT {Hierarchize({[Measures].[LoginUser Cnt]})} ON COLUMNS, {Hierarchize({[Time].[2012].[Q3].[09].[05]})} ON ROWS FROM [bridge-kpi]</t>
   </si>
@@ -474,10 +474,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>[Time].[2012].[Q3].[09].[05]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>mdx</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -487,6 +483,18 @@
   </si>
   <si>
     <t xml:space="preserve">   </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">   </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">   </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2012-09-05</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -691,7 +699,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -728,6 +736,9 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -763,7 +774,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -1024,24 +1034,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="87151360"/>
-        <c:axId val="87152896"/>
+        <c:axId val="84398848"/>
+        <c:axId val="84400384"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="87151360"/>
+        <c:axId val="84398848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87152896"/>
+        <c:crossAx val="84400384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="87152896"/>
+        <c:axId val="84400384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1049,14 +1059,13 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87151360"/>
+        <c:crossAx val="84398848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -1067,7 +1076,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1093,7 +1102,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -1354,24 +1362,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="87513344"/>
-        <c:axId val="87539712"/>
+        <c:axId val="86464768"/>
+        <c:axId val="86491136"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="87513344"/>
+        <c:axId val="86464768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87539712"/>
+        <c:crossAx val="86491136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="87539712"/>
+        <c:axId val="86491136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1379,14 +1387,13 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87513344"/>
+        <c:crossAx val="86464768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -1397,7 +1404,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1755,7 +1762,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:Q27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
@@ -1767,16 +1774,19 @@
     <col min="11" max="16384" width="9" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" ht="22.5" customHeight="1">
+    <row r="1" spans="2:17" ht="22.5" customHeight="1">
       <c r="B1" s="9" t="str">
         <f>"商桥KPI数据 - "&amp;_input!A3&amp;_input!A2</f>
         <v>商桥KPI数据 - 05日</v>
       </c>
       <c r="C1" s="9"/>
       <c r="D1" s="9"/>
-    </row>
-    <row r="2" spans="2:15" ht="6" customHeight="1"/>
-    <row r="3" spans="2:15">
+      <c r="Q1" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="2:17" ht="6" customHeight="1"/>
+    <row r="3" spans="2:17">
       <c r="B3" s="11" t="s">
         <v>85</v>
       </c>
@@ -1790,7 +1800,7 @@
       </c>
       <c r="L3" s="10"/>
     </row>
-    <row r="4" spans="2:15">
+    <row r="4" spans="2:17">
       <c r="B4" s="6" t="s">
         <v>82</v>
       </c>
@@ -1809,7 +1819,7 @@
       <c r="N4" s="8"/>
       <c r="O4" s="8"/>
     </row>
-    <row r="5" spans="2:15" ht="16.5" customHeight="1">
+    <row r="5" spans="2:17" ht="16.5" customHeight="1">
       <c r="B5" s="7" t="str">
         <f>_input!B2</f>
         <v>登陆用户量</v>
@@ -1859,16 +1869,21 @@
         <v>6438</v>
       </c>
     </row>
-    <row r="6" spans="2:15" ht="12" customHeight="1"/>
-    <row r="7" spans="2:15">
+    <row r="6" spans="2:17" ht="12" customHeight="1"/>
+    <row r="7" spans="2:17">
       <c r="B7" s="11" t="s">
         <v>86</v>
       </c>
       <c r="C7" s="11"/>
     </row>
-    <row r="27" spans="17:17">
+    <row r="26" spans="16:17">
+      <c r="P26" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="16:17">
       <c r="Q27" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -1892,7 +1907,7 @@
   </sheetPr>
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
@@ -1912,13 +1927,13 @@
         <v>87</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>96</v>
+      <c r="E1" s="12" t="s">
+        <v>101</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>95</v>
@@ -1958,7 +1973,7 @@
         <v>94</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rill-analysis: Add support conditionalformatting
</commit_message>
<xml_diff>
--- a/rill-analysis/rill-analysis-report-core/src/test/resources/nu/com/rill/analysis/report/excel/bridge_kpi.xlsx
+++ b/rill-analysis/rill-analysis-report-core/src/test/resources/nu/com/rill/analysis/report/excel/bridge_kpi.xlsx
@@ -170,7 +170,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="164">
   <si>
     <t>日</t>
   </si>
@@ -656,6 +656,46 @@
   </si>
   <si>
     <t>环比</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>每日登录商桥的客户数（主子去重）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>近3个月登录过商桥的客户数（主子去重）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>每日登录商桥的主账号数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>每日登录商桥的子帐号数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>连续5工作日登陆商桥的客户数（主子去重）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>连续5工作日登陆商桥的主账号数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>连续5工作日登陆商桥的子账号数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>每日在线沟通客户数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>每日有留言的客户数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>每日有在线沟通和留言的去重客户数</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -663,7 +703,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -727,8 +767,15 @@
       <family val="2"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color theme="4"/>
+      <name val="微软雅黑"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -783,8 +830,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="17">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -913,17 +966,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color theme="0" tint="-4.9989318521683403E-2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color theme="0" tint="-4.9989318521683403E-2"/>
@@ -1020,7 +1062,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1032,13 +1074,13 @@
     <xf numFmtId="10" fontId="7" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="6" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1053,31 +1095,19 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
@@ -1086,13 +1116,13 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="7" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1104,28 +1134,40 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="3" fontId="7" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="7" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="7" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1133,10 +1175,924 @@
     <cellStyle name="常规" xfId="0" builtinId="0"/>
     <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="96">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF31E382"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF31E382"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF31E382"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF31E382"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF31E382"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF31E382"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF31E382"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF31E382"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF31E382"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF31E382"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF31E382"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF31E382"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF31E382"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF31E382"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF31E382"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF31E382"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF31E382"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF31E382"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF31E382"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF31E382"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF31E382"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF31E382"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF31E382"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF31E382"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF31E382"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF31E382"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF31E382"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF31E382"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF31E382"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF31E382"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF31E382"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF31E382"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF31E382"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF31E382"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF31E382"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF31E382"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF31E382"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF31E382"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF31E382"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF31E382"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF31E382"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF31E382"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF31E382"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF31E382"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF31E382"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF31E382"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF31E382"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF31E382"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF31E382"/>
       <color rgb="FF4B97BD"/>
     </mruColors>
   </colors>
@@ -3692,24 +4648,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="42360832"/>
-        <c:axId val="42362368"/>
+        <c:axId val="72135040"/>
+        <c:axId val="72136576"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="42360832"/>
+        <c:axId val="72135040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="42362368"/>
+        <c:crossAx val="72136576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="42362368"/>
+        <c:axId val="72136576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3717,7 +4673,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="42360832"/>
+        <c:crossAx val="72135040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3730,7 +4686,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000002" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000002" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000255" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000255" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -6285,24 +7241,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="42422272"/>
-        <c:axId val="42423808"/>
+        <c:axId val="72360320"/>
+        <c:axId val="72361856"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="42422272"/>
+        <c:axId val="72360320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="42423808"/>
+        <c:crossAx val="72361856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="42423808"/>
+        <c:axId val="72361856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6310,20 +7266,19 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="#,##0" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="42422272"/>
+        <c:crossAx val="72360320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000222" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000222" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000278" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000278" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -6698,17 +7653,17 @@
   <sheetData>
     <row r="1" spans="1:31" ht="6.75" customHeight="1"/>
     <row r="2" spans="1:31" ht="16.5" customHeight="1">
-      <c r="B2" s="45" t="str">
+      <c r="B2" s="29" t="str">
         <f>"商桥KPI数据 - "&amp;_input!A3&amp;_input!A2</f>
         <v>商桥KPI数据 - 08日</v>
       </c>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
       <c r="J2" s="8"/>
       <c r="K2" s="8"/>
       <c r="L2" s="8"/>
@@ -6734,65 +7689,65 @@
     </row>
     <row r="3" spans="1:31" ht="16.5" customHeight="1"/>
     <row r="4" spans="1:31" ht="16.5" customHeight="1">
-      <c r="B4" s="44" t="s">
+      <c r="B4" s="30" t="s">
         <v>150</v>
       </c>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44"/>
-      <c r="F4" s="44"/>
-      <c r="G4" s="44"/>
-      <c r="H4" s="44"/>
-      <c r="I4" s="44"/>
-      <c r="J4" s="44"/>
-      <c r="L4" s="46"/>
-      <c r="M4" s="46"/>
-      <c r="N4" s="46"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="30"/>
+      <c r="L4" s="31"/>
+      <c r="M4" s="31"/>
+      <c r="N4" s="31"/>
     </row>
     <row r="5" spans="1:31" ht="16.5" customHeight="1">
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="32" t="s">
         <v>151</v>
       </c>
-      <c r="C5" s="37"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="36" t="s">
+      <c r="C5" s="33"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="32" t="s">
         <v>152</v>
       </c>
-      <c r="F5" s="37"/>
-      <c r="G5" s="38"/>
-      <c r="H5" s="36" t="s">
+      <c r="F5" s="33"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="32" t="s">
         <v>153</v>
       </c>
-      <c r="I5" s="37"/>
-      <c r="J5" s="38"/>
-      <c r="O5" s="43" t="s">
+      <c r="I5" s="33"/>
+      <c r="J5" s="34"/>
+      <c r="O5" s="39" t="s">
         <v>92</v>
       </c>
-      <c r="P5" s="43"/>
-      <c r="U5" s="43" t="s">
+      <c r="P5" s="39"/>
+      <c r="U5" s="39" t="s">
         <v>95</v>
       </c>
-      <c r="V5" s="43"/>
+      <c r="V5" s="39"/>
     </row>
     <row r="6" spans="1:31" ht="16.5" customHeight="1">
-      <c r="B6" s="41" t="str">
+      <c r="B6" s="35" t="str">
         <f>_input!B2</f>
         <v>用户登录量</v>
       </c>
-      <c r="C6" s="41"/>
-      <c r="D6" s="42"/>
-      <c r="E6" s="39">
+      <c r="C6" s="35"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="37">
         <f>_input!B3</f>
         <v>0</v>
       </c>
-      <c r="F6" s="40"/>
-      <c r="G6" s="40"/>
-      <c r="H6" s="33">
+      <c r="F6" s="38"/>
+      <c r="G6" s="38"/>
+      <c r="H6" s="40">
         <f>_input!J223</f>
         <v>0</v>
       </c>
-      <c r="I6" s="34"/>
-      <c r="J6" s="35"/>
+      <c r="I6" s="41"/>
+      <c r="J6" s="42"/>
       <c r="L6" s="10"/>
       <c r="M6" s="10"/>
       <c r="N6" s="11"/>
@@ -6839,20 +7794,22 @@
     </row>
     <row r="7" spans="1:31" ht="16.5" customHeight="1">
       <c r="A7" s="9"/>
-      <c r="B7" s="22"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="28"/>
-      <c r="H7" s="28"/>
-      <c r="I7" s="28"/>
-      <c r="J7" s="23"/>
-      <c r="L7" s="36" t="s">
+      <c r="B7" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="C7" s="43"/>
+      <c r="D7" s="43"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="43"/>
+      <c r="H7" s="43"/>
+      <c r="I7" s="43"/>
+      <c r="J7" s="44"/>
+      <c r="L7" s="32" t="s">
         <v>91</v>
       </c>
-      <c r="M7" s="37"/>
-      <c r="N7" s="38"/>
+      <c r="M7" s="33"/>
+      <c r="N7" s="34"/>
       <c r="O7" s="13">
         <f>_input!B7</f>
         <v>0</v>
@@ -6896,20 +7853,20 @@
     </row>
     <row r="8" spans="1:31" ht="16.5" customHeight="1">
       <c r="A8" s="9"/>
-      <c r="B8" s="25"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="25"/>
-      <c r="I8" s="25"/>
-      <c r="J8" s="26"/>
-      <c r="L8" s="36" t="s">
+      <c r="B8" s="45"/>
+      <c r="C8" s="45"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="45"/>
+      <c r="H8" s="45"/>
+      <c r="I8" s="45"/>
+      <c r="J8" s="46"/>
+      <c r="L8" s="32" t="s">
         <v>90</v>
       </c>
-      <c r="M8" s="37"/>
-      <c r="N8" s="38"/>
+      <c r="M8" s="33"/>
+      <c r="N8" s="34"/>
       <c r="O8" s="14">
         <f>_input!B8</f>
         <v>0</v>
@@ -6953,50 +7910,50 @@
     </row>
     <row r="9" spans="1:31" ht="6" customHeight="1">
       <c r="A9" s="9"/>
-      <c r="B9" s="28"/>
-      <c r="C9" s="28"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="28"/>
-      <c r="G9" s="28"/>
-      <c r="H9" s="28"/>
-      <c r="I9" s="28"/>
-      <c r="J9" s="23"/>
-      <c r="K9" s="28"/>
-      <c r="L9" s="28"/>
-      <c r="M9" s="28"/>
-      <c r="N9" s="28"/>
-      <c r="O9" s="28"/>
-      <c r="P9" s="28"/>
-      <c r="Q9" s="28"/>
-      <c r="R9" s="28"/>
-      <c r="S9" s="28"/>
-      <c r="T9" s="28"/>
-      <c r="U9" s="28"/>
-      <c r="V9" s="28"/>
-      <c r="W9" s="28"/>
-      <c r="X9" s="28"/>
-      <c r="Y9" s="28"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="24"/>
+      <c r="J9" s="22"/>
+      <c r="K9" s="24"/>
+      <c r="L9" s="24"/>
+      <c r="M9" s="24"/>
+      <c r="N9" s="24"/>
+      <c r="O9" s="24"/>
+      <c r="P9" s="24"/>
+      <c r="Q9" s="24"/>
+      <c r="R9" s="24"/>
+      <c r="S9" s="24"/>
+      <c r="T9" s="24"/>
+      <c r="U9" s="24"/>
+      <c r="V9" s="24"/>
+      <c r="W9" s="24"/>
+      <c r="X9" s="24"/>
+      <c r="Y9" s="24"/>
     </row>
     <row r="10" spans="1:31" ht="16.5" customHeight="1">
-      <c r="B10" s="41" t="str">
+      <c r="B10" s="35" t="str">
         <f>_input!B96</f>
         <v>使用量</v>
       </c>
-      <c r="C10" s="41"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="39">
+      <c r="C10" s="35"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="37">
         <f>_input!B97</f>
         <v>0</v>
       </c>
-      <c r="F10" s="40"/>
-      <c r="G10" s="40"/>
-      <c r="H10" s="33">
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="40">
         <f>_input!K223</f>
         <v>0</v>
       </c>
-      <c r="I10" s="34"/>
-      <c r="J10" s="35"/>
+      <c r="I10" s="41"/>
+      <c r="J10" s="42"/>
       <c r="L10" s="10"/>
       <c r="M10" s="10"/>
       <c r="N10" s="11"/>
@@ -7043,20 +8000,22 @@
     </row>
     <row r="11" spans="1:31" ht="16.5" customHeight="1">
       <c r="A11" s="9"/>
-      <c r="B11" s="22"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="28"/>
-      <c r="I11" s="28"/>
-      <c r="J11" s="23"/>
-      <c r="L11" s="36" t="s">
+      <c r="B11" s="43" t="s">
+        <v>155</v>
+      </c>
+      <c r="C11" s="43"/>
+      <c r="D11" s="43"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="43"/>
+      <c r="H11" s="43"/>
+      <c r="I11" s="43"/>
+      <c r="J11" s="44"/>
+      <c r="L11" s="32" t="s">
         <v>91</v>
       </c>
-      <c r="M11" s="37"/>
-      <c r="N11" s="38"/>
+      <c r="M11" s="33"/>
+      <c r="N11" s="34"/>
       <c r="O11" s="13">
         <f>_input!B101</f>
         <v>0</v>
@@ -7100,20 +8059,20 @@
     </row>
     <row r="12" spans="1:31" ht="16.5" customHeight="1">
       <c r="A12" s="9"/>
-      <c r="B12" s="25"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="25"/>
-      <c r="I12" s="25"/>
-      <c r="J12" s="26"/>
-      <c r="L12" s="36" t="s">
+      <c r="B12" s="43"/>
+      <c r="C12" s="43"/>
+      <c r="D12" s="43"/>
+      <c r="E12" s="43"/>
+      <c r="F12" s="43"/>
+      <c r="G12" s="43"/>
+      <c r="H12" s="43"/>
+      <c r="I12" s="43"/>
+      <c r="J12" s="44"/>
+      <c r="L12" s="32" t="s">
         <v>90</v>
       </c>
-      <c r="M12" s="37"/>
-      <c r="N12" s="38"/>
+      <c r="M12" s="33"/>
+      <c r="N12" s="34"/>
       <c r="O12" s="14">
         <f>_input!B102</f>
         <v>0</v>
@@ -7157,50 +8116,50 @@
     </row>
     <row r="13" spans="1:31" ht="6" customHeight="1">
       <c r="A13" s="9"/>
-      <c r="B13" s="28"/>
-      <c r="C13" s="28"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="28"/>
-      <c r="G13" s="28"/>
-      <c r="H13" s="28"/>
-      <c r="I13" s="28"/>
-      <c r="J13" s="23"/>
-      <c r="K13" s="28"/>
-      <c r="L13" s="28"/>
-      <c r="M13" s="28"/>
-      <c r="N13" s="28"/>
-      <c r="O13" s="28"/>
-      <c r="P13" s="28"/>
-      <c r="Q13" s="28"/>
-      <c r="R13" s="28"/>
-      <c r="S13" s="28"/>
-      <c r="T13" s="28"/>
-      <c r="U13" s="28"/>
-      <c r="V13" s="28"/>
-      <c r="W13" s="28"/>
-      <c r="X13" s="28"/>
-      <c r="Y13" s="28"/>
+      <c r="B13" s="24"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="24"/>
+      <c r="J13" s="22"/>
+      <c r="K13" s="24"/>
+      <c r="L13" s="24"/>
+      <c r="M13" s="24"/>
+      <c r="N13" s="24"/>
+      <c r="O13" s="24"/>
+      <c r="P13" s="24"/>
+      <c r="Q13" s="24"/>
+      <c r="R13" s="24"/>
+      <c r="S13" s="24"/>
+      <c r="T13" s="24"/>
+      <c r="U13" s="24"/>
+      <c r="V13" s="24"/>
+      <c r="W13" s="24"/>
+      <c r="X13" s="24"/>
+      <c r="Y13" s="24"/>
     </row>
     <row r="14" spans="1:31" ht="16.5" customHeight="1">
-      <c r="B14" s="41" t="str">
+      <c r="B14" s="35" t="str">
         <f>_input!B110</f>
         <v>主账号登录数</v>
       </c>
-      <c r="C14" s="41"/>
-      <c r="D14" s="42"/>
-      <c r="E14" s="39">
+      <c r="C14" s="35"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="37">
         <f>_input!B111</f>
         <v>0</v>
       </c>
-      <c r="F14" s="40"/>
-      <c r="G14" s="40"/>
-      <c r="H14" s="33">
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="40">
         <f>_input!H223</f>
         <v>0</v>
       </c>
-      <c r="I14" s="34"/>
-      <c r="J14" s="35"/>
+      <c r="I14" s="41"/>
+      <c r="J14" s="42"/>
       <c r="L14" s="10"/>
       <c r="M14" s="10"/>
       <c r="N14" s="11"/>
@@ -7247,20 +8206,22 @@
     </row>
     <row r="15" spans="1:31" ht="16.5" customHeight="1">
       <c r="A15" s="9"/>
-      <c r="B15" s="22"/>
-      <c r="C15" s="22"/>
-      <c r="D15" s="23"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="28"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="28"/>
-      <c r="I15" s="28"/>
-      <c r="J15" s="23"/>
-      <c r="L15" s="36" t="s">
+      <c r="B15" s="43" t="s">
+        <v>156</v>
+      </c>
+      <c r="C15" s="43"/>
+      <c r="D15" s="43"/>
+      <c r="E15" s="43"/>
+      <c r="F15" s="43"/>
+      <c r="G15" s="43"/>
+      <c r="H15" s="43"/>
+      <c r="I15" s="43"/>
+      <c r="J15" s="44"/>
+      <c r="L15" s="32" t="s">
         <v>91</v>
       </c>
-      <c r="M15" s="37"/>
-      <c r="N15" s="38"/>
+      <c r="M15" s="33"/>
+      <c r="N15" s="34"/>
       <c r="O15" s="13">
         <f>_input!B115</f>
         <v>0</v>
@@ -7304,20 +8265,20 @@
     </row>
     <row r="16" spans="1:31" ht="16.5" customHeight="1">
       <c r="A16" s="9"/>
-      <c r="B16" s="25"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="27"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="25"/>
-      <c r="H16" s="25"/>
-      <c r="I16" s="25"/>
-      <c r="J16" s="26"/>
-      <c r="L16" s="36" t="s">
+      <c r="B16" s="43"/>
+      <c r="C16" s="43"/>
+      <c r="D16" s="43"/>
+      <c r="E16" s="43"/>
+      <c r="F16" s="43"/>
+      <c r="G16" s="43"/>
+      <c r="H16" s="43"/>
+      <c r="I16" s="43"/>
+      <c r="J16" s="44"/>
+      <c r="L16" s="32" t="s">
         <v>90</v>
       </c>
-      <c r="M16" s="37"/>
-      <c r="N16" s="38"/>
+      <c r="M16" s="33"/>
+      <c r="N16" s="34"/>
       <c r="O16" s="14">
         <f>_input!B116</f>
         <v>0</v>
@@ -7361,50 +8322,50 @@
     </row>
     <row r="17" spans="1:25" ht="6" customHeight="1">
       <c r="A17" s="9"/>
-      <c r="B17" s="28"/>
-      <c r="C17" s="28"/>
-      <c r="D17" s="28"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="28"/>
-      <c r="G17" s="28"/>
-      <c r="H17" s="28"/>
-      <c r="I17" s="28"/>
-      <c r="J17" s="23"/>
-      <c r="K17" s="28"/>
-      <c r="L17" s="28"/>
-      <c r="M17" s="28"/>
-      <c r="N17" s="28"/>
-      <c r="O17" s="28"/>
-      <c r="P17" s="28"/>
-      <c r="Q17" s="28"/>
-      <c r="R17" s="28"/>
-      <c r="S17" s="28"/>
-      <c r="T17" s="28"/>
-      <c r="U17" s="28"/>
-      <c r="V17" s="28"/>
-      <c r="W17" s="28"/>
-      <c r="X17" s="28"/>
-      <c r="Y17" s="28"/>
+      <c r="B17" s="24"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="24"/>
+      <c r="I17" s="24"/>
+      <c r="J17" s="22"/>
+      <c r="K17" s="24"/>
+      <c r="L17" s="24"/>
+      <c r="M17" s="24"/>
+      <c r="N17" s="24"/>
+      <c r="O17" s="24"/>
+      <c r="P17" s="24"/>
+      <c r="Q17" s="24"/>
+      <c r="R17" s="24"/>
+      <c r="S17" s="24"/>
+      <c r="T17" s="24"/>
+      <c r="U17" s="24"/>
+      <c r="V17" s="24"/>
+      <c r="W17" s="24"/>
+      <c r="X17" s="24"/>
+      <c r="Y17" s="24"/>
     </row>
     <row r="18" spans="1:25" ht="16.5" customHeight="1">
-      <c r="B18" s="41" t="str">
+      <c r="B18" s="35" t="str">
         <f>_input!B124</f>
         <v>子账号登录数</v>
       </c>
-      <c r="C18" s="41"/>
-      <c r="D18" s="42"/>
-      <c r="E18" s="39">
+      <c r="C18" s="35"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="37">
         <f>_input!B125</f>
         <v>0</v>
       </c>
-      <c r="F18" s="40"/>
-      <c r="G18" s="40"/>
-      <c r="H18" s="33">
+      <c r="F18" s="38"/>
+      <c r="G18" s="38"/>
+      <c r="H18" s="40">
         <f>_input!I223</f>
         <v>0</v>
       </c>
-      <c r="I18" s="34"/>
-      <c r="J18" s="35"/>
+      <c r="I18" s="41"/>
+      <c r="J18" s="42"/>
       <c r="L18" s="10"/>
       <c r="M18" s="10"/>
       <c r="N18" s="11"/>
@@ -7451,20 +8412,22 @@
     </row>
     <row r="19" spans="1:25" ht="16.5" customHeight="1">
       <c r="A19" s="9"/>
-      <c r="B19" s="22"/>
-      <c r="C19" s="22"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="24"/>
-      <c r="F19" s="28"/>
-      <c r="G19" s="28"/>
-      <c r="H19" s="28"/>
-      <c r="I19" s="28"/>
-      <c r="J19" s="23"/>
-      <c r="L19" s="36" t="s">
+      <c r="B19" s="43" t="s">
+        <v>157</v>
+      </c>
+      <c r="C19" s="43"/>
+      <c r="D19" s="43"/>
+      <c r="E19" s="43"/>
+      <c r="F19" s="43"/>
+      <c r="G19" s="43"/>
+      <c r="H19" s="43"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="44"/>
+      <c r="L19" s="32" t="s">
         <v>91</v>
       </c>
-      <c r="M19" s="37"/>
-      <c r="N19" s="38"/>
+      <c r="M19" s="33"/>
+      <c r="N19" s="34"/>
       <c r="O19" s="13">
         <f>_input!B129</f>
         <v>0</v>
@@ -7508,20 +8471,20 @@
     </row>
     <row r="20" spans="1:25" ht="16.5" customHeight="1">
       <c r="A20" s="9"/>
-      <c r="B20" s="25"/>
-      <c r="C20" s="25"/>
-      <c r="D20" s="26"/>
-      <c r="E20" s="27"/>
-      <c r="F20" s="25"/>
-      <c r="G20" s="25"/>
-      <c r="H20" s="25"/>
-      <c r="I20" s="25"/>
-      <c r="J20" s="26"/>
-      <c r="L20" s="36" t="s">
+      <c r="B20" s="43"/>
+      <c r="C20" s="43"/>
+      <c r="D20" s="43"/>
+      <c r="E20" s="43"/>
+      <c r="F20" s="43"/>
+      <c r="G20" s="43"/>
+      <c r="H20" s="43"/>
+      <c r="I20" s="43"/>
+      <c r="J20" s="44"/>
+      <c r="L20" s="32" t="s">
         <v>90</v>
       </c>
-      <c r="M20" s="37"/>
-      <c r="N20" s="38"/>
+      <c r="M20" s="33"/>
+      <c r="N20" s="34"/>
       <c r="O20" s="14">
         <f>_input!B130</f>
         <v>0</v>
@@ -7565,50 +8528,50 @@
     </row>
     <row r="21" spans="1:25" ht="6" customHeight="1">
       <c r="A21" s="9"/>
-      <c r="B21" s="28"/>
-      <c r="C21" s="28"/>
-      <c r="D21" s="28"/>
-      <c r="E21" s="28"/>
-      <c r="F21" s="28"/>
-      <c r="G21" s="28"/>
-      <c r="H21" s="28"/>
-      <c r="I21" s="28"/>
-      <c r="J21" s="23"/>
-      <c r="K21" s="28"/>
-      <c r="L21" s="28"/>
-      <c r="M21" s="28"/>
-      <c r="N21" s="28"/>
-      <c r="O21" s="28"/>
-      <c r="P21" s="28"/>
-      <c r="Q21" s="28"/>
-      <c r="R21" s="28"/>
-      <c r="S21" s="28"/>
-      <c r="T21" s="28"/>
-      <c r="U21" s="28"/>
-      <c r="V21" s="28"/>
-      <c r="W21" s="28"/>
-      <c r="X21" s="28"/>
-      <c r="Y21" s="28"/>
+      <c r="B21" s="24"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="24"/>
+      <c r="H21" s="24"/>
+      <c r="I21" s="24"/>
+      <c r="J21" s="22"/>
+      <c r="K21" s="24"/>
+      <c r="L21" s="24"/>
+      <c r="M21" s="24"/>
+      <c r="N21" s="24"/>
+      <c r="O21" s="24"/>
+      <c r="P21" s="24"/>
+      <c r="Q21" s="24"/>
+      <c r="R21" s="24"/>
+      <c r="S21" s="24"/>
+      <c r="T21" s="24"/>
+      <c r="U21" s="24"/>
+      <c r="V21" s="24"/>
+      <c r="W21" s="24"/>
+      <c r="X21" s="24"/>
+      <c r="Y21" s="24"/>
     </row>
     <row r="22" spans="1:25" ht="16.5" customHeight="1">
-      <c r="B22" s="41" t="str">
+      <c r="B22" s="35" t="str">
         <f>_input!B138</f>
         <v>有商机客户数</v>
       </c>
-      <c r="C22" s="41"/>
-      <c r="D22" s="42"/>
-      <c r="E22" s="39">
+      <c r="C22" s="35"/>
+      <c r="D22" s="36"/>
+      <c r="E22" s="37">
         <f>_input!B139</f>
         <v>0</v>
       </c>
-      <c r="F22" s="40"/>
-      <c r="G22" s="40"/>
-      <c r="H22" s="33">
+      <c r="F22" s="38"/>
+      <c r="G22" s="38"/>
+      <c r="H22" s="40">
         <f>_input!G223</f>
         <v>0</v>
       </c>
-      <c r="I22" s="34"/>
-      <c r="J22" s="35"/>
+      <c r="I22" s="41"/>
+      <c r="J22" s="42"/>
       <c r="L22" s="10"/>
       <c r="M22" s="10"/>
       <c r="N22" s="11"/>
@@ -7655,20 +8618,22 @@
     </row>
     <row r="23" spans="1:25" ht="16.5" customHeight="1">
       <c r="A23" s="9"/>
-      <c r="B23" s="22"/>
-      <c r="C23" s="22"/>
-      <c r="D23" s="23"/>
-      <c r="E23" s="24"/>
-      <c r="F23" s="28"/>
-      <c r="G23" s="28"/>
-      <c r="H23" s="28"/>
-      <c r="I23" s="28"/>
-      <c r="J23" s="23"/>
-      <c r="L23" s="36" t="s">
+      <c r="B23" s="43" t="s">
+        <v>163</v>
+      </c>
+      <c r="C23" s="43"/>
+      <c r="D23" s="43"/>
+      <c r="E23" s="43"/>
+      <c r="F23" s="43"/>
+      <c r="G23" s="43"/>
+      <c r="H23" s="43"/>
+      <c r="I23" s="43"/>
+      <c r="J23" s="44"/>
+      <c r="L23" s="32" t="s">
         <v>91</v>
       </c>
-      <c r="M23" s="37"/>
-      <c r="N23" s="38"/>
+      <c r="M23" s="33"/>
+      <c r="N23" s="34"/>
       <c r="O23" s="13">
         <f>_input!B143</f>
         <v>0</v>
@@ -7712,20 +8677,20 @@
     </row>
     <row r="24" spans="1:25" ht="16.5" customHeight="1">
       <c r="A24" s="9"/>
-      <c r="B24" s="25"/>
-      <c r="C24" s="25"/>
-      <c r="D24" s="26"/>
-      <c r="E24" s="27"/>
-      <c r="F24" s="25"/>
-      <c r="G24" s="25"/>
-      <c r="H24" s="25"/>
-      <c r="I24" s="25"/>
-      <c r="J24" s="26"/>
-      <c r="L24" s="36" t="s">
+      <c r="B24" s="43"/>
+      <c r="C24" s="43"/>
+      <c r="D24" s="43"/>
+      <c r="E24" s="43"/>
+      <c r="F24" s="43"/>
+      <c r="G24" s="43"/>
+      <c r="H24" s="43"/>
+      <c r="I24" s="43"/>
+      <c r="J24" s="44"/>
+      <c r="L24" s="32" t="s">
         <v>90</v>
       </c>
-      <c r="M24" s="37"/>
-      <c r="N24" s="38"/>
+      <c r="M24" s="33"/>
+      <c r="N24" s="34"/>
       <c r="O24" s="14">
         <f>_input!B144</f>
         <v>0</v>
@@ -7769,55 +8734,55 @@
     </row>
     <row r="25" spans="1:25" ht="6" customHeight="1">
       <c r="A25" s="9"/>
-      <c r="B25" s="28"/>
-      <c r="C25" s="28"/>
-      <c r="D25" s="23"/>
-      <c r="E25" s="24"/>
-      <c r="F25" s="28"/>
-      <c r="G25" s="28"/>
-      <c r="H25" s="28"/>
-      <c r="I25" s="28"/>
-      <c r="J25" s="23"/>
-      <c r="K25" s="28"/>
-      <c r="L25" s="28"/>
-      <c r="M25" s="28"/>
-      <c r="N25" s="28"/>
-      <c r="O25" s="28"/>
-      <c r="P25" s="28"/>
-      <c r="Q25" s="28"/>
-      <c r="R25" s="28"/>
-      <c r="S25" s="28"/>
-      <c r="T25" s="28"/>
-      <c r="U25" s="28"/>
-      <c r="V25" s="28"/>
-      <c r="W25" s="28"/>
-      <c r="X25" s="28"/>
-      <c r="Y25" s="28"/>
+      <c r="B25" s="24"/>
+      <c r="C25" s="24"/>
+      <c r="D25" s="22"/>
+      <c r="E25" s="23"/>
+      <c r="F25" s="24"/>
+      <c r="G25" s="24"/>
+      <c r="H25" s="24"/>
+      <c r="I25" s="24"/>
+      <c r="J25" s="22"/>
+      <c r="K25" s="24"/>
+      <c r="L25" s="24"/>
+      <c r="M25" s="24"/>
+      <c r="N25" s="24"/>
+      <c r="O25" s="24"/>
+      <c r="P25" s="24"/>
+      <c r="Q25" s="24"/>
+      <c r="R25" s="24"/>
+      <c r="S25" s="24"/>
+      <c r="T25" s="24"/>
+      <c r="U25" s="24"/>
+      <c r="V25" s="24"/>
+      <c r="W25" s="24"/>
+      <c r="X25" s="24"/>
+      <c r="Y25" s="24"/>
     </row>
     <row r="26" spans="1:25" ht="16.5" customHeight="1">
       <c r="A26" s="9"/>
-      <c r="B26" s="41" t="str">
+      <c r="B26" s="35" t="str">
         <f>_input!B152</f>
         <v>有沟通客户数</v>
       </c>
-      <c r="C26" s="41"/>
-      <c r="D26" s="42"/>
-      <c r="E26" s="39">
+      <c r="C26" s="35"/>
+      <c r="D26" s="36"/>
+      <c r="E26" s="37">
         <f>_input!B153</f>
         <v>0</v>
       </c>
-      <c r="F26" s="40"/>
-      <c r="G26" s="40"/>
-      <c r="H26" s="33">
+      <c r="F26" s="38"/>
+      <c r="G26" s="38"/>
+      <c r="H26" s="40">
         <f>_input!E223</f>
         <v>0</v>
       </c>
-      <c r="I26" s="34"/>
-      <c r="J26" s="35"/>
-      <c r="K26" s="28"/>
-      <c r="L26" s="28"/>
-      <c r="M26" s="28"/>
-      <c r="N26" s="28"/>
+      <c r="I26" s="41"/>
+      <c r="J26" s="42"/>
+      <c r="K26" s="24"/>
+      <c r="L26" s="24"/>
+      <c r="M26" s="24"/>
+      <c r="N26" s="24"/>
       <c r="O26" s="12" t="str">
         <f>_input!B156</f>
         <v>机械设备</v>
@@ -7861,20 +8826,22 @@
     </row>
     <row r="27" spans="1:25" ht="16.5" customHeight="1">
       <c r="A27" s="9"/>
-      <c r="B27" s="22"/>
-      <c r="C27" s="22"/>
-      <c r="D27" s="23"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="28"/>
-      <c r="G27" s="28"/>
-      <c r="H27" s="28"/>
-      <c r="I27" s="28"/>
-      <c r="J27" s="23"/>
-      <c r="L27" s="36" t="s">
+      <c r="B27" s="43" t="s">
+        <v>161</v>
+      </c>
+      <c r="C27" s="43"/>
+      <c r="D27" s="43"/>
+      <c r="E27" s="43"/>
+      <c r="F27" s="43"/>
+      <c r="G27" s="43"/>
+      <c r="H27" s="43"/>
+      <c r="I27" s="43"/>
+      <c r="J27" s="44"/>
+      <c r="L27" s="32" t="s">
         <v>91</v>
       </c>
-      <c r="M27" s="37"/>
-      <c r="N27" s="38"/>
+      <c r="M27" s="33"/>
+      <c r="N27" s="34"/>
       <c r="O27" s="13">
         <f>_input!B157</f>
         <v>0</v>
@@ -7918,20 +8885,20 @@
     </row>
     <row r="28" spans="1:25" ht="16.5" customHeight="1">
       <c r="A28" s="9"/>
-      <c r="B28" s="25"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="26"/>
-      <c r="E28" s="27"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="25"/>
-      <c r="J28" s="26"/>
-      <c r="L28" s="36" t="s">
+      <c r="B28" s="43"/>
+      <c r="C28" s="43"/>
+      <c r="D28" s="43"/>
+      <c r="E28" s="43"/>
+      <c r="F28" s="43"/>
+      <c r="G28" s="43"/>
+      <c r="H28" s="43"/>
+      <c r="I28" s="43"/>
+      <c r="J28" s="44"/>
+      <c r="L28" s="32" t="s">
         <v>90</v>
       </c>
-      <c r="M28" s="37"/>
-      <c r="N28" s="38"/>
+      <c r="M28" s="33"/>
+      <c r="N28" s="34"/>
       <c r="O28" s="14">
         <f>_input!B158</f>
         <v>0</v>
@@ -7975,50 +8942,50 @@
     </row>
     <row r="29" spans="1:25" ht="6" customHeight="1">
       <c r="A29" s="9"/>
-      <c r="B29" s="31"/>
-      <c r="C29" s="31"/>
-      <c r="D29" s="29"/>
-      <c r="E29" s="30"/>
-      <c r="F29" s="31"/>
-      <c r="G29" s="31"/>
-      <c r="H29" s="31"/>
-      <c r="I29" s="31"/>
-      <c r="J29" s="29"/>
-      <c r="K29" s="28"/>
-      <c r="L29" s="28"/>
-      <c r="M29" s="28"/>
-      <c r="N29" s="28"/>
-      <c r="O29" s="28"/>
-      <c r="P29" s="28"/>
-      <c r="Q29" s="28"/>
-      <c r="R29" s="28"/>
-      <c r="S29" s="28"/>
-      <c r="T29" s="28"/>
-      <c r="U29" s="28"/>
-      <c r="V29" s="28"/>
-      <c r="W29" s="28"/>
-      <c r="X29" s="28"/>
-      <c r="Y29" s="28"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="25"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="27"/>
+      <c r="I29" s="27"/>
+      <c r="J29" s="25"/>
+      <c r="K29" s="24"/>
+      <c r="L29" s="24"/>
+      <c r="M29" s="24"/>
+      <c r="N29" s="24"/>
+      <c r="O29" s="24"/>
+      <c r="P29" s="24"/>
+      <c r="Q29" s="24"/>
+      <c r="R29" s="24"/>
+      <c r="S29" s="24"/>
+      <c r="T29" s="24"/>
+      <c r="U29" s="24"/>
+      <c r="V29" s="24"/>
+      <c r="W29" s="24"/>
+      <c r="X29" s="24"/>
+      <c r="Y29" s="24"/>
     </row>
     <row r="30" spans="1:25" ht="16.5" customHeight="1">
-      <c r="B30" s="41" t="str">
+      <c r="B30" s="35" t="str">
         <f>_input!B166</f>
         <v>有留言客户数</v>
       </c>
-      <c r="C30" s="41"/>
-      <c r="D30" s="42"/>
-      <c r="E30" s="39">
+      <c r="C30" s="35"/>
+      <c r="D30" s="36"/>
+      <c r="E30" s="37">
         <f>_input!B167</f>
         <v>0</v>
       </c>
-      <c r="F30" s="40"/>
-      <c r="G30" s="40"/>
-      <c r="H30" s="33">
+      <c r="F30" s="38"/>
+      <c r="G30" s="38"/>
+      <c r="H30" s="40">
         <f>_input!F223</f>
         <v>0</v>
       </c>
-      <c r="I30" s="34"/>
-      <c r="J30" s="35"/>
+      <c r="I30" s="41"/>
+      <c r="J30" s="42"/>
       <c r="L30" s="10"/>
       <c r="M30" s="10"/>
       <c r="N30" s="11"/>
@@ -8065,20 +9032,22 @@
     </row>
     <row r="31" spans="1:25" ht="16.5" customHeight="1">
       <c r="A31" s="9"/>
-      <c r="B31" s="22"/>
-      <c r="C31" s="22"/>
-      <c r="D31" s="23"/>
-      <c r="E31" s="24"/>
-      <c r="F31" s="28"/>
-      <c r="G31" s="28"/>
-      <c r="H31" s="28"/>
-      <c r="I31" s="28"/>
-      <c r="J31" s="23"/>
-      <c r="L31" s="36" t="s">
+      <c r="B31" s="43" t="s">
+        <v>162</v>
+      </c>
+      <c r="C31" s="43"/>
+      <c r="D31" s="43"/>
+      <c r="E31" s="43"/>
+      <c r="F31" s="43"/>
+      <c r="G31" s="43"/>
+      <c r="H31" s="43"/>
+      <c r="I31" s="43"/>
+      <c r="J31" s="44"/>
+      <c r="L31" s="32" t="s">
         <v>91</v>
       </c>
-      <c r="M31" s="37"/>
-      <c r="N31" s="38"/>
+      <c r="M31" s="33"/>
+      <c r="N31" s="34"/>
       <c r="O31" s="13">
         <f>_input!B171</f>
         <v>0</v>
@@ -8122,20 +9091,20 @@
     </row>
     <row r="32" spans="1:25" ht="16.5" customHeight="1">
       <c r="A32" s="9"/>
-      <c r="B32" s="25"/>
-      <c r="C32" s="25"/>
-      <c r="D32" s="26"/>
-      <c r="E32" s="27"/>
-      <c r="F32" s="25"/>
-      <c r="G32" s="25"/>
-      <c r="H32" s="25"/>
-      <c r="I32" s="25"/>
-      <c r="J32" s="26"/>
-      <c r="L32" s="36" t="s">
+      <c r="B32" s="43"/>
+      <c r="C32" s="43"/>
+      <c r="D32" s="43"/>
+      <c r="E32" s="43"/>
+      <c r="F32" s="43"/>
+      <c r="G32" s="43"/>
+      <c r="H32" s="43"/>
+      <c r="I32" s="43"/>
+      <c r="J32" s="44"/>
+      <c r="L32" s="32" t="s">
         <v>90</v>
       </c>
-      <c r="M32" s="37"/>
-      <c r="N32" s="38"/>
+      <c r="M32" s="33"/>
+      <c r="N32" s="34"/>
       <c r="O32" s="14">
         <f>_input!B172</f>
         <v>0</v>
@@ -8179,50 +9148,50 @@
     </row>
     <row r="33" spans="1:25" ht="6" customHeight="1">
       <c r="A33" s="9"/>
-      <c r="B33" s="31"/>
-      <c r="C33" s="31"/>
-      <c r="D33" s="29"/>
-      <c r="E33" s="30"/>
-      <c r="F33" s="31"/>
-      <c r="G33" s="31"/>
-      <c r="H33" s="31"/>
-      <c r="I33" s="31"/>
-      <c r="J33" s="29"/>
-      <c r="K33" s="28"/>
-      <c r="L33" s="28"/>
-      <c r="M33" s="28"/>
-      <c r="N33" s="28"/>
-      <c r="O33" s="28"/>
-      <c r="P33" s="28"/>
-      <c r="Q33" s="28"/>
-      <c r="R33" s="28"/>
-      <c r="S33" s="28"/>
-      <c r="T33" s="28"/>
-      <c r="U33" s="28"/>
-      <c r="V33" s="28"/>
-      <c r="W33" s="28"/>
-      <c r="X33" s="28"/>
-      <c r="Y33" s="28"/>
+      <c r="B33" s="27"/>
+      <c r="C33" s="27"/>
+      <c r="D33" s="25"/>
+      <c r="E33" s="26"/>
+      <c r="F33" s="27"/>
+      <c r="G33" s="27"/>
+      <c r="H33" s="27"/>
+      <c r="I33" s="27"/>
+      <c r="J33" s="25"/>
+      <c r="K33" s="24"/>
+      <c r="L33" s="24"/>
+      <c r="M33" s="24"/>
+      <c r="N33" s="24"/>
+      <c r="O33" s="24"/>
+      <c r="P33" s="24"/>
+      <c r="Q33" s="24"/>
+      <c r="R33" s="24"/>
+      <c r="S33" s="24"/>
+      <c r="T33" s="24"/>
+      <c r="U33" s="24"/>
+      <c r="V33" s="24"/>
+      <c r="W33" s="24"/>
+      <c r="X33" s="24"/>
+      <c r="Y33" s="24"/>
     </row>
     <row r="34" spans="1:25" ht="16.5" customHeight="1">
-      <c r="B34" s="41" t="str">
+      <c r="B34" s="35" t="str">
         <f>_input!B180</f>
         <v>活跃主账号数</v>
       </c>
-      <c r="C34" s="41"/>
-      <c r="D34" s="42"/>
-      <c r="E34" s="39">
+      <c r="C34" s="35"/>
+      <c r="D34" s="36"/>
+      <c r="E34" s="37">
         <f>_input!B181</f>
         <v>0</v>
       </c>
-      <c r="F34" s="40"/>
-      <c r="G34" s="40"/>
-      <c r="H34" s="33">
+      <c r="F34" s="38"/>
+      <c r="G34" s="38"/>
+      <c r="H34" s="40">
         <f>_input!B223</f>
         <v>0</v>
       </c>
-      <c r="I34" s="34"/>
-      <c r="J34" s="35"/>
+      <c r="I34" s="41"/>
+      <c r="J34" s="42"/>
       <c r="L34" s="10"/>
       <c r="M34" s="10"/>
       <c r="N34" s="11"/>
@@ -8269,20 +9238,22 @@
     </row>
     <row r="35" spans="1:25" ht="16.5" customHeight="1">
       <c r="A35" s="9"/>
-      <c r="B35" s="22"/>
-      <c r="C35" s="22"/>
-      <c r="D35" s="23"/>
-      <c r="E35" s="24"/>
-      <c r="F35" s="28"/>
-      <c r="G35" s="28"/>
-      <c r="H35" s="28"/>
-      <c r="I35" s="28"/>
-      <c r="J35" s="23"/>
-      <c r="L35" s="36" t="s">
+      <c r="B35" s="43" t="s">
+        <v>159</v>
+      </c>
+      <c r="C35" s="43"/>
+      <c r="D35" s="43"/>
+      <c r="E35" s="43"/>
+      <c r="F35" s="43"/>
+      <c r="G35" s="43"/>
+      <c r="H35" s="43"/>
+      <c r="I35" s="43"/>
+      <c r="J35" s="44"/>
+      <c r="L35" s="32" t="s">
         <v>91</v>
       </c>
-      <c r="M35" s="37"/>
-      <c r="N35" s="38"/>
+      <c r="M35" s="33"/>
+      <c r="N35" s="34"/>
       <c r="O35" s="13">
         <f>_input!B185</f>
         <v>0</v>
@@ -8326,20 +9297,20 @@
     </row>
     <row r="36" spans="1:25" ht="16.5" customHeight="1">
       <c r="A36" s="9"/>
-      <c r="B36" s="25"/>
-      <c r="C36" s="25"/>
-      <c r="D36" s="26"/>
-      <c r="E36" s="27"/>
-      <c r="F36" s="25"/>
-      <c r="G36" s="25"/>
-      <c r="H36" s="25"/>
-      <c r="I36" s="25"/>
-      <c r="J36" s="26"/>
-      <c r="L36" s="36" t="s">
+      <c r="B36" s="43"/>
+      <c r="C36" s="43"/>
+      <c r="D36" s="43"/>
+      <c r="E36" s="43"/>
+      <c r="F36" s="43"/>
+      <c r="G36" s="43"/>
+      <c r="H36" s="43"/>
+      <c r="I36" s="43"/>
+      <c r="J36" s="44"/>
+      <c r="L36" s="32" t="s">
         <v>90</v>
       </c>
-      <c r="M36" s="37"/>
-      <c r="N36" s="38"/>
+      <c r="M36" s="33"/>
+      <c r="N36" s="34"/>
       <c r="O36" s="14">
         <f>_input!B186</f>
         <v>0</v>
@@ -8383,50 +9354,50 @@
     </row>
     <row r="37" spans="1:25" ht="6" customHeight="1">
       <c r="A37" s="9"/>
-      <c r="B37" s="31"/>
-      <c r="C37" s="31"/>
-      <c r="D37" s="29"/>
-      <c r="E37" s="30"/>
-      <c r="F37" s="31"/>
-      <c r="G37" s="31"/>
-      <c r="H37" s="31"/>
-      <c r="I37" s="31"/>
-      <c r="J37" s="29"/>
-      <c r="K37" s="28"/>
-      <c r="L37" s="28"/>
-      <c r="M37" s="28"/>
-      <c r="N37" s="28"/>
-      <c r="O37" s="28"/>
-      <c r="P37" s="28"/>
-      <c r="Q37" s="28"/>
-      <c r="R37" s="28"/>
-      <c r="S37" s="28"/>
-      <c r="T37" s="28"/>
-      <c r="U37" s="28"/>
-      <c r="V37" s="28"/>
-      <c r="W37" s="28"/>
-      <c r="X37" s="28"/>
-      <c r="Y37" s="28"/>
+      <c r="B37" s="27"/>
+      <c r="C37" s="27"/>
+      <c r="D37" s="25"/>
+      <c r="E37" s="26"/>
+      <c r="F37" s="27"/>
+      <c r="G37" s="27"/>
+      <c r="H37" s="27"/>
+      <c r="I37" s="27"/>
+      <c r="J37" s="25"/>
+      <c r="K37" s="24"/>
+      <c r="L37" s="24"/>
+      <c r="M37" s="24"/>
+      <c r="N37" s="24"/>
+      <c r="O37" s="24"/>
+      <c r="P37" s="24"/>
+      <c r="Q37" s="24"/>
+      <c r="R37" s="24"/>
+      <c r="S37" s="24"/>
+      <c r="T37" s="24"/>
+      <c r="U37" s="24"/>
+      <c r="V37" s="24"/>
+      <c r="W37" s="24"/>
+      <c r="X37" s="24"/>
+      <c r="Y37" s="24"/>
     </row>
     <row r="38" spans="1:25" ht="16.5" customHeight="1">
-      <c r="B38" s="41" t="str">
+      <c r="B38" s="35" t="str">
         <f>_input!B194</f>
         <v>活跃子账号数</v>
       </c>
-      <c r="C38" s="41"/>
-      <c r="D38" s="42"/>
-      <c r="E38" s="39">
+      <c r="C38" s="35"/>
+      <c r="D38" s="36"/>
+      <c r="E38" s="37">
         <f>_input!B195</f>
         <v>0</v>
       </c>
-      <c r="F38" s="40"/>
-      <c r="G38" s="40"/>
-      <c r="H38" s="33">
+      <c r="F38" s="38"/>
+      <c r="G38" s="38"/>
+      <c r="H38" s="40">
         <f>_input!C223</f>
         <v>0</v>
       </c>
-      <c r="I38" s="34"/>
-      <c r="J38" s="35"/>
+      <c r="I38" s="41"/>
+      <c r="J38" s="42"/>
       <c r="L38" s="10"/>
       <c r="M38" s="10"/>
       <c r="N38" s="11"/>
@@ -8473,20 +9444,22 @@
     </row>
     <row r="39" spans="1:25" ht="16.5" customHeight="1">
       <c r="A39" s="9"/>
-      <c r="B39" s="22"/>
-      <c r="C39" s="22"/>
-      <c r="D39" s="23"/>
-      <c r="E39" s="24"/>
-      <c r="F39" s="28"/>
-      <c r="G39" s="28"/>
-      <c r="H39" s="28"/>
-      <c r="I39" s="28"/>
-      <c r="J39" s="23"/>
-      <c r="L39" s="36" t="s">
+      <c r="B39" s="43" t="s">
+        <v>160</v>
+      </c>
+      <c r="C39" s="43"/>
+      <c r="D39" s="43"/>
+      <c r="E39" s="43"/>
+      <c r="F39" s="43"/>
+      <c r="G39" s="43"/>
+      <c r="H39" s="43"/>
+      <c r="I39" s="43"/>
+      <c r="J39" s="44"/>
+      <c r="L39" s="32" t="s">
         <v>91</v>
       </c>
-      <c r="M39" s="37"/>
-      <c r="N39" s="38"/>
+      <c r="M39" s="33"/>
+      <c r="N39" s="34"/>
       <c r="O39" s="13">
         <f>_input!B199</f>
         <v>0</v>
@@ -8530,20 +9503,20 @@
     </row>
     <row r="40" spans="1:25" ht="16.5" customHeight="1">
       <c r="A40" s="9"/>
-      <c r="B40" s="25"/>
-      <c r="C40" s="25"/>
-      <c r="D40" s="26"/>
-      <c r="E40" s="27"/>
-      <c r="F40" s="25"/>
-      <c r="G40" s="25"/>
-      <c r="H40" s="25"/>
-      <c r="I40" s="25"/>
-      <c r="J40" s="26"/>
-      <c r="L40" s="36" t="s">
+      <c r="B40" s="43"/>
+      <c r="C40" s="43"/>
+      <c r="D40" s="43"/>
+      <c r="E40" s="43"/>
+      <c r="F40" s="43"/>
+      <c r="G40" s="43"/>
+      <c r="H40" s="43"/>
+      <c r="I40" s="43"/>
+      <c r="J40" s="44"/>
+      <c r="L40" s="32" t="s">
         <v>90</v>
       </c>
-      <c r="M40" s="37"/>
-      <c r="N40" s="38"/>
+      <c r="M40" s="33"/>
+      <c r="N40" s="34"/>
       <c r="O40" s="14">
         <f>_input!B200</f>
         <v>0</v>
@@ -8587,50 +9560,50 @@
     </row>
     <row r="41" spans="1:25" ht="6" customHeight="1">
       <c r="A41" s="9"/>
-      <c r="B41" s="31"/>
-      <c r="C41" s="31"/>
-      <c r="D41" s="29"/>
-      <c r="E41" s="30"/>
-      <c r="F41" s="31"/>
-      <c r="G41" s="31"/>
-      <c r="H41" s="31"/>
-      <c r="I41" s="31"/>
-      <c r="J41" s="29"/>
-      <c r="K41" s="28"/>
-      <c r="L41" s="28"/>
-      <c r="M41" s="28"/>
-      <c r="N41" s="28"/>
-      <c r="O41" s="28"/>
-      <c r="P41" s="28"/>
-      <c r="Q41" s="28"/>
-      <c r="R41" s="28"/>
-      <c r="S41" s="28"/>
-      <c r="T41" s="28"/>
-      <c r="U41" s="28"/>
-      <c r="V41" s="28"/>
-      <c r="W41" s="28"/>
-      <c r="X41" s="28"/>
-      <c r="Y41" s="28"/>
+      <c r="B41" s="27"/>
+      <c r="C41" s="27"/>
+      <c r="D41" s="25"/>
+      <c r="E41" s="26"/>
+      <c r="F41" s="27"/>
+      <c r="G41" s="27"/>
+      <c r="H41" s="27"/>
+      <c r="I41" s="27"/>
+      <c r="J41" s="25"/>
+      <c r="K41" s="24"/>
+      <c r="L41" s="24"/>
+      <c r="M41" s="24"/>
+      <c r="N41" s="24"/>
+      <c r="O41" s="24"/>
+      <c r="P41" s="24"/>
+      <c r="Q41" s="24"/>
+      <c r="R41" s="24"/>
+      <c r="S41" s="24"/>
+      <c r="T41" s="24"/>
+      <c r="U41" s="24"/>
+      <c r="V41" s="24"/>
+      <c r="W41" s="24"/>
+      <c r="X41" s="24"/>
+      <c r="Y41" s="24"/>
     </row>
     <row r="42" spans="1:25" ht="16.5" customHeight="1">
-      <c r="B42" s="41" t="str">
+      <c r="B42" s="35" t="str">
         <f>_input!B208</f>
         <v>活跃用户数</v>
       </c>
-      <c r="C42" s="41"/>
-      <c r="D42" s="42"/>
-      <c r="E42" s="39">
+      <c r="C42" s="35"/>
+      <c r="D42" s="36"/>
+      <c r="E42" s="37">
         <f>_input!B209</f>
         <v>0</v>
       </c>
-      <c r="F42" s="40"/>
-      <c r="G42" s="40"/>
-      <c r="H42" s="33">
+      <c r="F42" s="38"/>
+      <c r="G42" s="38"/>
+      <c r="H42" s="40">
         <f>_input!D223</f>
         <v>0</v>
       </c>
-      <c r="I42" s="34"/>
-      <c r="J42" s="35"/>
+      <c r="I42" s="41"/>
+      <c r="J42" s="42"/>
       <c r="L42" s="10"/>
       <c r="M42" s="10"/>
       <c r="N42" s="11"/>
@@ -8677,20 +9650,22 @@
     </row>
     <row r="43" spans="1:25" ht="16.5" customHeight="1">
       <c r="A43" s="9"/>
-      <c r="B43" s="22"/>
-      <c r="C43" s="22"/>
-      <c r="D43" s="23"/>
-      <c r="E43" s="24"/>
-      <c r="F43" s="28"/>
-      <c r="G43" s="28"/>
-      <c r="H43" s="28"/>
-      <c r="I43" s="28"/>
-      <c r="J43" s="23"/>
-      <c r="L43" s="36" t="s">
+      <c r="B43" s="43" t="s">
+        <v>158</v>
+      </c>
+      <c r="C43" s="43"/>
+      <c r="D43" s="43"/>
+      <c r="E43" s="43"/>
+      <c r="F43" s="43"/>
+      <c r="G43" s="43"/>
+      <c r="H43" s="43"/>
+      <c r="I43" s="43"/>
+      <c r="J43" s="44"/>
+      <c r="L43" s="32" t="s">
         <v>91</v>
       </c>
-      <c r="M43" s="37"/>
-      <c r="N43" s="38"/>
+      <c r="M43" s="33"/>
+      <c r="N43" s="34"/>
       <c r="O43" s="13">
         <f>_input!B213</f>
         <v>0</v>
@@ -8734,20 +9709,20 @@
     </row>
     <row r="44" spans="1:25" ht="16.5" customHeight="1">
       <c r="A44" s="9"/>
-      <c r="B44" s="25"/>
-      <c r="C44" s="25"/>
-      <c r="D44" s="26"/>
-      <c r="E44" s="27"/>
-      <c r="F44" s="25"/>
-      <c r="G44" s="25"/>
-      <c r="H44" s="25"/>
-      <c r="I44" s="25"/>
-      <c r="J44" s="26"/>
-      <c r="L44" s="36" t="s">
+      <c r="B44" s="43"/>
+      <c r="C44" s="43"/>
+      <c r="D44" s="43"/>
+      <c r="E44" s="43"/>
+      <c r="F44" s="43"/>
+      <c r="G44" s="43"/>
+      <c r="H44" s="43"/>
+      <c r="I44" s="43"/>
+      <c r="J44" s="44"/>
+      <c r="L44" s="32" t="s">
         <v>90</v>
       </c>
-      <c r="M44" s="37"/>
-      <c r="N44" s="38"/>
+      <c r="M44" s="33"/>
+      <c r="N44" s="34"/>
       <c r="O44" s="14">
         <f>_input!B214</f>
         <v>0</v>
@@ -8790,30 +9765,30 @@
       </c>
     </row>
     <row r="46" spans="1:25">
-      <c r="B46" s="44" t="s">
+      <c r="B46" s="30" t="s">
         <v>93</v>
       </c>
-      <c r="C46" s="44"/>
-      <c r="D46" s="44"/>
-      <c r="E46" s="44"/>
-      <c r="F46" s="44"/>
-      <c r="G46" s="44"/>
-      <c r="H46" s="44"/>
-      <c r="I46" s="44"/>
-      <c r="J46" s="44"/>
+      <c r="C46" s="30"/>
+      <c r="D46" s="30"/>
+      <c r="E46" s="30"/>
+      <c r="F46" s="30"/>
+      <c r="G46" s="30"/>
+      <c r="H46" s="30"/>
+      <c r="I46" s="30"/>
+      <c r="J46" s="30"/>
     </row>
     <row r="61" spans="2:10">
-      <c r="B61" s="44" t="s">
+      <c r="B61" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="C61" s="44"/>
-      <c r="D61" s="44"/>
-      <c r="E61" s="44"/>
-      <c r="F61" s="44"/>
-      <c r="G61" s="44"/>
-      <c r="H61" s="44"/>
-      <c r="I61" s="44"/>
-      <c r="J61" s="44"/>
+      <c r="C61" s="30"/>
+      <c r="D61" s="30"/>
+      <c r="E61" s="30"/>
+      <c r="F61" s="30"/>
+      <c r="G61" s="30"/>
+      <c r="H61" s="30"/>
+      <c r="I61" s="30"/>
+      <c r="J61" s="30"/>
     </row>
     <row r="75" spans="26:26">
       <c r="Z75" s="5" t="s">
@@ -8821,10 +9796,71 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="60">
+  <mergeCells count="80">
+    <mergeCell ref="B27:J27"/>
+    <mergeCell ref="B28:J28"/>
+    <mergeCell ref="B31:J31"/>
+    <mergeCell ref="B32:J32"/>
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="B39:J39"/>
+    <mergeCell ref="B40:J40"/>
+    <mergeCell ref="H34:J34"/>
+    <mergeCell ref="E38:G38"/>
+    <mergeCell ref="H38:J38"/>
+    <mergeCell ref="B43:J43"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="H5:J5"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="E10:G10"/>
+    <mergeCell ref="H10:J10"/>
+    <mergeCell ref="B11:J11"/>
+    <mergeCell ref="B12:J12"/>
+    <mergeCell ref="B15:J15"/>
+    <mergeCell ref="B7:J7"/>
+    <mergeCell ref="B8:J8"/>
+    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="E30:G30"/>
+    <mergeCell ref="H30:J30"/>
+    <mergeCell ref="E34:G34"/>
+    <mergeCell ref="L44:N44"/>
+    <mergeCell ref="L36:N36"/>
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="L27:N27"/>
+    <mergeCell ref="L28:N28"/>
+    <mergeCell ref="L31:N31"/>
+    <mergeCell ref="L32:N32"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="B35:J35"/>
+    <mergeCell ref="B36:J36"/>
+    <mergeCell ref="L43:N43"/>
+    <mergeCell ref="L39:N39"/>
+    <mergeCell ref="L40:N40"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="H26:J26"/>
+    <mergeCell ref="B16:J16"/>
+    <mergeCell ref="B19:J19"/>
+    <mergeCell ref="B20:J20"/>
+    <mergeCell ref="B23:J23"/>
+    <mergeCell ref="B24:J24"/>
     <mergeCell ref="U5:V5"/>
     <mergeCell ref="O5:P5"/>
     <mergeCell ref="B61:J61"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="H14:J14"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B44:J44"/>
+    <mergeCell ref="L35:N35"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="E18:G18"/>
+    <mergeCell ref="H18:J18"/>
+    <mergeCell ref="L20:N20"/>
+    <mergeCell ref="E22:G22"/>
+    <mergeCell ref="H22:J22"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="B46:J46"/>
     <mergeCell ref="B4:J4"/>
@@ -8838,52 +9874,91 @@
     <mergeCell ref="L23:N23"/>
     <mergeCell ref="L24:N24"/>
     <mergeCell ref="B22:D22"/>
-    <mergeCell ref="L35:N35"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="E18:G18"/>
-    <mergeCell ref="H18:J18"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="H14:J14"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="L20:N20"/>
-    <mergeCell ref="E22:G22"/>
-    <mergeCell ref="H22:J22"/>
-    <mergeCell ref="E26:G26"/>
-    <mergeCell ref="H26:J26"/>
     <mergeCell ref="L12:N12"/>
     <mergeCell ref="L11:N11"/>
-    <mergeCell ref="L44:N44"/>
-    <mergeCell ref="L36:N36"/>
-    <mergeCell ref="B42:D42"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="L27:N27"/>
-    <mergeCell ref="L28:N28"/>
-    <mergeCell ref="L31:N31"/>
-    <mergeCell ref="L32:N32"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="E14:G14"/>
-    <mergeCell ref="L43:N43"/>
-    <mergeCell ref="L39:N39"/>
-    <mergeCell ref="L40:N40"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="H5:J5"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="H10:J10"/>
-    <mergeCell ref="E30:G30"/>
-    <mergeCell ref="H30:J30"/>
-    <mergeCell ref="E34:G34"/>
-    <mergeCell ref="H34:J34"/>
-    <mergeCell ref="E38:G38"/>
-    <mergeCell ref="H38:J38"/>
-    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="E26:G26"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="H6:J6">
+    <cfRule type="cellIs" dxfId="95" priority="40" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="76" priority="50" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H10:J10">
+    <cfRule type="cellIs" dxfId="35" priority="17" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="34" priority="18" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H14:J14">
+    <cfRule type="cellIs" dxfId="31" priority="15" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="16" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H18:J18">
+    <cfRule type="cellIs" dxfId="27" priority="13" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="26" priority="14" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H22:J22">
+    <cfRule type="cellIs" dxfId="23" priority="11" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="12" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H26:J26">
+    <cfRule type="cellIs" dxfId="19" priority="9" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="10" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H30:J30">
+    <cfRule type="cellIs" dxfId="15" priority="7" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="8" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H34:J34">
+    <cfRule type="cellIs" dxfId="11" priority="5" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="6" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H38:J38">
+    <cfRule type="cellIs" dxfId="7" priority="3" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H42:J42">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>